<commit_message>
Fixing Table 5 panel 2
</commit_message>
<xml_diff>
--- a/results/table5_panel1.xlsx
+++ b/results/table5_panel1.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\w18d541\Documents\GitHub\lpdt\results\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -82,8 +87,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,10 +140,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -146,6 +154,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -192,7 +208,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -224,9 +240,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -258,6 +275,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -433,14 +451,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:F7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="1">
         <v>0</v>
       </c>
@@ -457,7 +477,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -477,103 +497,103 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>6.22</v>
       </c>
-      <c r="C3">
-        <v>8.199999999999999</v>
-      </c>
-      <c r="D3">
+      <c r="C3" s="2">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="D3" s="2">
         <v>7.65</v>
       </c>
-      <c r="E3">
-        <v>9.529999999999999</v>
-      </c>
-      <c r="F3">
+      <c r="E3" s="2">
+        <v>9.5299999999999994</v>
+      </c>
+      <c r="F3" s="2">
         <v>7.92</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>6.41</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>7.7</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>7.86</v>
       </c>
-      <c r="E5">
-        <v>9.130000000000001</v>
-      </c>
-      <c r="F5">
+      <c r="E5" s="2">
+        <v>9.1300000000000008</v>
+      </c>
+      <c r="F5" s="2">
         <v>7.65</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>1465</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>6915</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <v>3330</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <v>3290</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2">
         <v>6733</v>
       </c>
     </row>

</xml_diff>